<commit_message>
:books: best_fx to all executions for boxplots + median tests
</commit_message>
<xml_diff>
--- a/Execucoes Gerais/novo_final_GraficoFinal_Artigo.xlsx
+++ b/Execucoes Gerais/novo_final_GraficoFinal_Artigo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19485" windowHeight="7860" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="19485" windowHeight="7860" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="GRI" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <t>GEOreal2_P_DS</t>
   </si>
   <si>
-    <t>AA-GEO2real</t>
+    <t>sAA-GEO2real</t>
   </si>
   <si>
     <t>============================================================================</t>
@@ -96,10 +96,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -134,49 +134,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,24 +148,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,31 +173,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,7 +218,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,13 +271,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +355,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,37 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,109 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,6 +465,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -474,11 +504,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,17 +543,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,186 +562,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1775,7 +1775,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2994,7 +2994,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4271,7 +4271,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5552,7 +5552,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7134,7 +7134,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8659,7 +8659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10183,7 +10183,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -11708,7 +11708,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13233,7 +13233,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14451,7 +14451,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15725,7 +15725,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17002,7 +17002,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AA-GEO2real</c:v>
+                  <c:v>sAA-GEO2real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -24492,182 +24492,121 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685165</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="1371600" y="542925"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="5486400" y="542925"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>685165</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="1371600" y="3257550"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="5486400" y="3257550"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="9601200" y="542925"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="9601200" y="3257550"/>
-        <a:ext cx="4114800" cy="2743200"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="Group 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1370965" y="542925"/>
+          <a:ext cx="12344400" cy="5457825"/>
+          <a:chOff x="2141" y="835"/>
+          <a:chExt cx="19376" cy="8513"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="2" name="Chart 1"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="2141" y="835"/>
+          <a:ext cx="6459" cy="4277"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="8600" y="835"/>
+          <a:ext cx="6459" cy="4277"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="4" name="Chart 3"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="2141" y="5070"/>
+          <a:ext cx="6459" cy="4278"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="5" name="Chart 4"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="8600" y="5070"/>
+          <a:ext cx="6459" cy="4278"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="6" name="Chart 5"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="15059" y="835"/>
+          <a:ext cx="6459" cy="4277"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:graphicFrame>
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="7" name="Chart 6"/>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="15059" y="5070"/>
+          <a:ext cx="6459" cy="4278"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -27958,7 +27897,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -28794,7 +28733,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -29629,7 +29568,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -30464,7 +30403,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -31299,7 +31238,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -32133,8 +32072,8 @@
   <sheetPr/>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -32973,8 +32912,8 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>

</xml_diff>